<commit_message>
updated changes and use of IDE for delete test
</commit_message>
<xml_diff>
--- a/TestFolder/TalkShopTestCases.xlsx
+++ b/TestFolder/TalkShopTestCases.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\Documents\CIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnazzaro\Documents\GitHub\talkshop\TestFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Number</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>SearchForSpeaker</t>
+  </si>
+  <si>
+    <t>DeleteAccount</t>
+  </si>
+  <si>
+    <t>A user should be able to delete their account and try to login once it has been deleted</t>
   </si>
 </sst>
 </file>
@@ -194,10 +200,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -510,55 +516,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" customWidth="1"/>
-    <col min="2" max="2" width="72.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="72.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -578,7 +584,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -598,7 +604,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -618,7 +624,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -638,7 +644,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -658,7 +664,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -678,7 +684,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -698,7 +704,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -718,7 +724,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -738,7 +744,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -755,6 +761,26 @@
         <v>42101</v>
       </c>
       <c r="F13">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14">
+        <v>11</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="1">
+        <v>42102</v>
+      </c>
+      <c r="F14">
         <v>0.6</v>
       </c>
     </row>

</xml_diff>